<commit_message>
Termino do Documento visao
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/Planejamento e Controle do epCafe.xlsx
+++ b/Gerenciamento de Projeto/Planejamento e Controle do epCafe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Documents/Java/grupo-6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Documents/Java/grupo-6/Gerenciamento de Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{8E4C21FE-B85A-8246-8C29-6A1642DED4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC72D3B-4A9A-B048-9D84-2EA778A1F6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" tabRatio="797" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="10" r:id="rId1"/>
@@ -4332,7 +4332,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="47" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4655,12 +4655,6 @@
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="18">
@@ -5492,6 +5486,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5574,21 +5571,6 @@
     <xf numFmtId="0" fontId="28" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5610,6 +5592,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5621,6 +5606,18 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5669,9 +5666,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -5957,7 +5951,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6049,34 +6043,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.5500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.6000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.75</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8499999999999996</c:v>
+                  <c:v>5.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8999999999999997</c:v>
+                  <c:v>3.7999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.94999999999999973</c:v>
+                  <c:v>1.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -6461,7 +6455,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6553,34 +6547,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.5500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.6000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.75</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8499999999999996</c:v>
+                  <c:v>5.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8999999999999997</c:v>
+                  <c:v>3.7999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.94999999999999973</c:v>
+                  <c:v>1.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -6965,7 +6959,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7057,34 +7051,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.5500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.6000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.75</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8499999999999996</c:v>
+                  <c:v>5.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8999999999999997</c:v>
+                  <c:v>3.7999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.94999999999999973</c:v>
+                  <c:v>1.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -7469,7 +7463,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7561,34 +7555,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.5500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.6000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.75</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8499999999999996</c:v>
+                  <c:v>5.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8999999999999997</c:v>
+                  <c:v>3.7999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.94999999999999973</c:v>
+                  <c:v>1.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -7973,7 +7967,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8065,34 +8059,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.5500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.6000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.75</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8499999999999996</c:v>
+                  <c:v>5.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8999999999999997</c:v>
+                  <c:v>3.7999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.94999999999999973</c:v>
+                  <c:v>1.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -8477,7 +8471,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8569,34 +8563,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.5500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.6000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.75</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8499999999999996</c:v>
+                  <c:v>5.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8999999999999997</c:v>
+                  <c:v>3.7999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.94999999999999973</c:v>
+                  <c:v>1.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -13469,7 +13463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -13481,18 +13475,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="145" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
     </row>
     <row r="2" spans="1:3" ht="23" x14ac:dyDescent="0.2">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="146" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -13512,7 +13506,7 @@
       <c r="B4" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="C4" s="202" t="s">
+      <c r="C4" s="144" t="s">
         <v>256</v>
       </c>
     </row>
@@ -13523,7 +13517,7 @@
       <c r="B5" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C5" s="202" t="s">
+      <c r="C5" s="144" t="s">
         <v>254</v>
       </c>
     </row>
@@ -13534,7 +13528,7 @@
       <c r="B6" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="202" t="s">
+      <c r="C6" s="144" t="s">
         <v>254</v>
       </c>
     </row>
@@ -13545,7 +13539,7 @@
       <c r="B7" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="C7" s="202" t="s">
+      <c r="C7" s="144" t="s">
         <v>256</v>
       </c>
     </row>
@@ -13556,7 +13550,7 @@
       <c r="B8" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="C8" s="202" t="s">
+      <c r="C8" s="144" t="s">
         <v>255</v>
       </c>
     </row>
@@ -13627,7 +13621,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13684,7 +13678,7 @@
         <v>196</v>
       </c>
       <c r="B2" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -13702,7 +13696,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -13720,7 +13714,7 @@
         <v>193</v>
       </c>
       <c r="B4" s="15">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -13738,7 +13732,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="15">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -13756,7 +13750,7 @@
         <v>198</v>
       </c>
       <c r="B6" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -13774,7 +13768,7 @@
         <v>203</v>
       </c>
       <c r="B7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -13849,7 +13843,7 @@
       </c>
       <c r="B12" s="37">
         <f>SUM(B2:B11)</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C12" s="37" t="str">
         <f>IF(SUM(C2:C11)&gt;0,B12-SUM(C2:C11), "")</f>
@@ -13899,43 +13893,43 @@
       </c>
       <c r="B13" s="34">
         <f>B12</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C13" s="35">
         <f>B13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>21.6</v>
+        <v>43.2</v>
       </c>
       <c r="D13" s="35">
         <f t="shared" ref="D13:L13" si="1">C13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>19.200000000000003</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="E13" s="35">
         <f t="shared" si="1"/>
-        <v>16.800000000000004</v>
+        <v>33.600000000000009</v>
       </c>
       <c r="F13" s="35">
         <f t="shared" si="1"/>
-        <v>14.400000000000004</v>
+        <v>28.800000000000008</v>
       </c>
       <c r="G13" s="35">
         <f t="shared" si="1"/>
-        <v>12.000000000000004</v>
+        <v>24.000000000000007</v>
       </c>
       <c r="H13" s="35">
         <f t="shared" si="1"/>
-        <v>9.6000000000000032</v>
+        <v>19.200000000000006</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" si="1"/>
-        <v>7.2000000000000028</v>
+        <v>14.400000000000006</v>
       </c>
       <c r="J13" s="35">
         <f t="shared" si="1"/>
-        <v>4.8000000000000025</v>
+        <v>9.600000000000005</v>
       </c>
       <c r="K13" s="35">
         <f t="shared" si="1"/>
-        <v>2.4000000000000026</v>
+        <v>4.8000000000000052</v>
       </c>
       <c r="L13" s="35">
         <f t="shared" si="1"/>
@@ -13948,47 +13942,47 @@
       </c>
       <c r="B14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="C14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="D14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="E14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="F14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="G14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="H14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="I14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="J14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="K14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="L14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -14046,7 +14040,7 @@
       </c>
       <c r="B16" s="43">
         <f>Planejamento!B8</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>12</v>
@@ -14072,7 +14066,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14129,7 +14123,7 @@
         <v>196</v>
       </c>
       <c r="B2" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -14147,7 +14141,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -14165,7 +14159,7 @@
         <v>193</v>
       </c>
       <c r="B4" s="15">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -14183,7 +14177,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="15">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -14201,7 +14195,7 @@
         <v>198</v>
       </c>
       <c r="B6" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -14219,7 +14213,7 @@
         <v>203</v>
       </c>
       <c r="B7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -14294,7 +14288,7 @@
       </c>
       <c r="B12" s="37">
         <f>SUM(B2:B11)</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C12" s="37" t="str">
         <f>IF(SUM(C2:C11)&gt;0,B12-SUM(C2:C11), "")</f>
@@ -14344,43 +14338,43 @@
       </c>
       <c r="B13" s="34">
         <f>B12</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C13" s="35">
         <f>B13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>21.6</v>
+        <v>43.2</v>
       </c>
       <c r="D13" s="35">
         <f t="shared" ref="D13:L13" si="1">C13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>19.200000000000003</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="E13" s="35">
         <f t="shared" si="1"/>
-        <v>16.800000000000004</v>
+        <v>33.600000000000009</v>
       </c>
       <c r="F13" s="35">
         <f t="shared" si="1"/>
-        <v>14.400000000000004</v>
+        <v>28.800000000000008</v>
       </c>
       <c r="G13" s="35">
         <f t="shared" si="1"/>
-        <v>12.000000000000004</v>
+        <v>24.000000000000007</v>
       </c>
       <c r="H13" s="35">
         <f t="shared" si="1"/>
-        <v>9.6000000000000032</v>
+        <v>19.200000000000006</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" si="1"/>
-        <v>7.2000000000000028</v>
+        <v>14.400000000000006</v>
       </c>
       <c r="J13" s="35">
         <f t="shared" si="1"/>
-        <v>4.8000000000000025</v>
+        <v>9.600000000000005</v>
       </c>
       <c r="K13" s="35">
         <f t="shared" si="1"/>
-        <v>2.4000000000000026</v>
+        <v>4.8000000000000052</v>
       </c>
       <c r="L13" s="35">
         <f t="shared" si="1"/>
@@ -14393,47 +14387,47 @@
       </c>
       <c r="B14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="C14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="D14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="E14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="F14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="G14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="H14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="I14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="J14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="K14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="L14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -14491,7 +14485,7 @@
       </c>
       <c r="B16" s="43">
         <f>Planejamento!B8</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>12</v>
@@ -14517,7 +14511,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14574,7 +14568,7 @@
         <v>196</v>
       </c>
       <c r="B2" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -14592,7 +14586,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -14610,7 +14604,7 @@
         <v>193</v>
       </c>
       <c r="B4" s="15">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -14628,7 +14622,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="15">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -14646,7 +14640,7 @@
         <v>198</v>
       </c>
       <c r="B6" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -14664,7 +14658,7 @@
         <v>203</v>
       </c>
       <c r="B7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -14739,7 +14733,7 @@
       </c>
       <c r="B12" s="37">
         <f>SUM(B2:B11)</f>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C12" s="37" t="str">
         <f>IF(SUM(C2:C11)&gt;0,B12-SUM(C2:C11), "")</f>
@@ -14789,47 +14783,47 @@
       </c>
       <c r="B13" s="34">
         <f>B12</f>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C13" s="35">
         <f>B13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>32.4</v>
+        <v>64.8</v>
       </c>
       <c r="D13" s="35">
         <f t="shared" ref="D13:L13" si="1">C13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>28.799999999999997</v>
+        <v>57.599999999999994</v>
       </c>
       <c r="E13" s="35">
         <f t="shared" si="1"/>
-        <v>25.199999999999996</v>
+        <v>50.399999999999991</v>
       </c>
       <c r="F13" s="35">
         <f t="shared" si="1"/>
-        <v>21.599999999999994</v>
+        <v>43.199999999999989</v>
       </c>
       <c r="G13" s="35">
         <f t="shared" si="1"/>
-        <v>17.999999999999993</v>
+        <v>35.999999999999986</v>
       </c>
       <c r="H13" s="35">
         <f t="shared" si="1"/>
-        <v>14.399999999999993</v>
+        <v>28.799999999999986</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" si="1"/>
-        <v>10.799999999999994</v>
+        <v>21.599999999999987</v>
       </c>
       <c r="J13" s="35">
         <f t="shared" si="1"/>
-        <v>7.199999999999994</v>
+        <v>14.399999999999988</v>
       </c>
       <c r="K13" s="35">
         <f t="shared" si="1"/>
-        <v>3.5999999999999939</v>
+        <v>7.1999999999999877</v>
       </c>
       <c r="L13" s="35">
         <f t="shared" si="1"/>
-        <v>-6.2172489379008766E-15</v>
+        <v>-1.2434497875801753E-14</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -14838,47 +14832,47 @@
       </c>
       <c r="B14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="C14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="D14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="E14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="F14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="G14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="H14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="I14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="J14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="K14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="L14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -14936,7 +14930,7 @@
       </c>
       <c r="B16" s="43">
         <f>Planejamento!B8</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>12</v>
@@ -14984,116 +14978,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="54" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="195" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="194"/>
-      <c r="D1" s="194"/>
-      <c r="E1" s="194"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="194"/>
-      <c r="H1" s="194"/>
-      <c r="I1" s="194"/>
-      <c r="J1" s="194"/>
-      <c r="K1" s="194"/>
-      <c r="L1" s="194"/>
-      <c r="M1" s="194"/>
-      <c r="N1" s="194"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="195"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
     </row>
     <row r="2" spans="1:23" s="98" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="195" t="s">
+      <c r="A2" s="196" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="195"/>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="195"/>
+      <c r="B2" s="196"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="196"/>
+      <c r="G2" s="196"/>
+      <c r="H2" s="196"/>
+      <c r="I2" s="196"/>
+      <c r="J2" s="196"/>
+      <c r="K2" s="196"/>
+      <c r="L2" s="196"/>
+      <c r="M2" s="196"/>
+      <c r="N2" s="196"/>
     </row>
     <row r="3" spans="1:23" s="98" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="196" t="s">
+      <c r="A3" s="197" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="196"/>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="196"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="N3" s="196"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="197"/>
     </row>
     <row r="4" spans="1:23" s="98" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="197" t="s">
+      <c r="A4" s="198" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="197"/>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="197"/>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197"/>
-      <c r="I4" s="197"/>
-      <c r="J4" s="197"/>
-      <c r="K4" s="197"/>
-      <c r="L4" s="197"/>
-      <c r="M4" s="197"/>
-      <c r="N4" s="197"/>
+      <c r="B4" s="198"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="198"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="198"/>
+      <c r="K4" s="198"/>
+      <c r="L4" s="198"/>
+      <c r="M4" s="198"/>
+      <c r="N4" s="198"/>
     </row>
     <row r="5" spans="1:23" s="98" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="198" t="s">
+      <c r="A5" s="199" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="198"/>
-      <c r="C5" s="198"/>
-      <c r="D5" s="198"/>
-      <c r="E5" s="198"/>
-      <c r="F5" s="198"/>
-      <c r="G5" s="198"/>
-      <c r="H5" s="198"/>
-      <c r="I5" s="198"/>
-      <c r="J5" s="198"/>
-      <c r="K5" s="198"/>
-      <c r="L5" s="198"/>
-      <c r="M5" s="198"/>
-      <c r="N5" s="198"/>
+      <c r="B5" s="199"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="199"/>
+      <c r="E5" s="199"/>
+      <c r="F5" s="199"/>
+      <c r="G5" s="199"/>
+      <c r="H5" s="199"/>
+      <c r="I5" s="199"/>
+      <c r="J5" s="199"/>
+      <c r="K5" s="199"/>
+      <c r="L5" s="199"/>
+      <c r="M5" s="199"/>
+      <c r="N5" s="199"/>
     </row>
     <row r="6" spans="1:23" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.15">
-      <c r="A7" s="192" t="s">
+      <c r="A7" s="193" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="193"/>
-      <c r="D7" s="192" t="s">
+      <c r="B7" s="194"/>
+      <c r="D7" s="193" t="s">
         <v>173</v>
       </c>
-      <c r="E7" s="193"/>
-      <c r="G7" s="188" t="s">
+      <c r="E7" s="194"/>
+      <c r="G7" s="189" t="s">
         <v>140</v>
       </c>
-      <c r="H7" s="188"/>
-      <c r="I7" s="188"/>
-      <c r="J7" s="188"/>
-      <c r="K7" s="188"/>
-      <c r="M7" s="192" t="s">
+      <c r="H7" s="189"/>
+      <c r="I7" s="189"/>
+      <c r="J7" s="189"/>
+      <c r="K7" s="189"/>
+      <c r="M7" s="193" t="s">
         <v>174</v>
       </c>
-      <c r="N7" s="193"/>
+      <c r="N7" s="194"/>
     </row>
     <row r="8" spans="1:23" s="22" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="99" t="s">
@@ -15193,13 +15187,13 @@
       <c r="B11" s="101"/>
       <c r="D11" s="97"/>
       <c r="E11" s="101"/>
-      <c r="G11" s="188" t="s">
+      <c r="G11" s="189" t="s">
         <v>145</v>
       </c>
-      <c r="H11" s="188"/>
-      <c r="I11" s="188"/>
-      <c r="J11" s="188"/>
-      <c r="K11" s="188"/>
+      <c r="H11" s="189"/>
+      <c r="I11" s="189"/>
+      <c r="J11" s="189"/>
+      <c r="K11" s="189"/>
       <c r="M11" s="103" t="s">
         <v>160</v>
       </c>
@@ -15302,12 +15296,12 @@
       <c r="B16" s="101"/>
       <c r="D16" s="97"/>
       <c r="E16" s="101"/>
-      <c r="G16" s="189" t="s">
+      <c r="G16" s="190" t="s">
         <v>149</v>
       </c>
-      <c r="H16" s="190"/>
-      <c r="I16" s="190"/>
-      <c r="J16" s="191"/>
+      <c r="H16" s="191"/>
+      <c r="I16" s="191"/>
+      <c r="J16" s="192"/>
       <c r="K16" s="102">
         <f>SUM(K9,K10,K13,K14,K15)</f>
         <v>14</v>
@@ -15447,7 +15441,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15469,42 +15463,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="195" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="194"/>
-      <c r="D1" s="194"/>
-      <c r="E1" s="194"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="194"/>
-      <c r="H1" s="194"/>
-      <c r="I1" s="194"/>
-      <c r="J1" s="194"/>
-      <c r="K1" s="194"/>
-      <c r="L1" s="194"/>
-      <c r="M1" s="194"/>
-      <c r="N1" s="194"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="195"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
     </row>
     <row r="2" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="201" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="E3" s="187" t="s">
+      <c r="B3" s="201"/>
+      <c r="C3" s="201"/>
+      <c r="E3" s="188" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="187"/>
-      <c r="G3" s="187"/>
-      <c r="H3" s="187"/>
-      <c r="I3" s="187"/>
-      <c r="J3" s="187"/>
-      <c r="K3" s="187"/>
-      <c r="L3" s="187"/>
-      <c r="M3" s="187"/>
-      <c r="N3" s="187"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
+      <c r="I3" s="188"/>
+      <c r="J3" s="188"/>
+      <c r="K3" s="188"/>
+      <c r="L3" s="188"/>
+      <c r="M3" s="188"/>
+      <c r="N3" s="188"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -15517,25 +15511,25 @@
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="201" t="s">
+      <c r="E4" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="199" t="s">
+      <c r="F4" s="200" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="199"/>
-      <c r="H4" s="199" t="s">
+      <c r="G4" s="200"/>
+      <c r="H4" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="199"/>
-      <c r="J4" s="199" t="s">
+      <c r="I4" s="200"/>
+      <c r="J4" s="200" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="199"/>
-      <c r="L4" s="199" t="s">
+      <c r="K4" s="200"/>
+      <c r="L4" s="200" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="199"/>
+      <c r="M4" s="200"/>
       <c r="N4" s="115"/>
     </row>
     <row r="5" spans="1:14" ht="19" x14ac:dyDescent="0.25">
@@ -15548,23 +15542,23 @@
       <c r="C5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="201"/>
-      <c r="F5" s="199" t="s">
+      <c r="E5" s="202"/>
+      <c r="F5" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="199"/>
-      <c r="H5" s="199" t="s">
+      <c r="G5" s="200"/>
+      <c r="H5" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="199"/>
-      <c r="J5" s="199" t="s">
+      <c r="I5" s="200"/>
+      <c r="J5" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="199"/>
-      <c r="L5" s="199" t="s">
+      <c r="K5" s="200"/>
+      <c r="L5" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="199"/>
+      <c r="M5" s="200"/>
       <c r="N5" s="27" t="s">
         <v>186</v>
       </c>
@@ -15580,7 +15574,7 @@
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="201"/>
+      <c r="E6" s="202"/>
       <c r="F6" s="111">
         <f>B6*G6</f>
         <v>8.6450000000000014</v>
@@ -16012,11 +16006,11 @@
       <c r="N15" s="50"/>
     </row>
     <row r="16" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="200" t="s">
+      <c r="A16" s="201" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="200"/>
-      <c r="C16" s="200"/>
+      <c r="B16" s="201"/>
+      <c r="C16" s="201"/>
       <c r="E16" s="27" t="s">
         <v>187</v>
       </c>
@@ -16181,8 +16175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -16201,38 +16195,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="157" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="F1" s="149" t="s">
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="F1" s="150" t="s">
         <v>219</v>
       </c>
-      <c r="G1" s="150"/>
-      <c r="H1" s="150"/>
-      <c r="I1" s="150"/>
-      <c r="J1" s="150"/>
-      <c r="K1" s="150"/>
-      <c r="L1" s="150"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="151"/>
+      <c r="K1" s="151"/>
+      <c r="L1" s="151"/>
     </row>
     <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="152" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="152"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="F2" s="153" t="s">
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="F2" s="154" t="s">
         <v>243</v>
       </c>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
+      <c r="L2" s="155"/>
     </row>
     <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="133" t="s">
@@ -16253,20 +16247,20 @@
       <c r="G3" s="134" t="s">
         <v>217</v>
       </c>
-      <c r="H3" s="155" t="s">
+      <c r="H3" s="156" t="s">
         <v>219</v>
       </c>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
-      <c r="K3" s="155"/>
-      <c r="L3" s="155"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="156"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
     </row>
     <row r="4" spans="1:12" ht="26" x14ac:dyDescent="0.15">
-      <c r="A4" s="146" t="s">
+      <c r="A4" s="147" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="147"/>
-      <c r="C4" s="148"/>
+      <c r="B4" s="148"/>
+      <c r="C4" s="149"/>
       <c r="D4" s="126" t="s">
         <v>12</v>
       </c>
@@ -16465,11 +16459,11 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="146" t="s">
+      <c r="A11" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="147"/>
-      <c r="C11" s="148"/>
+      <c r="B11" s="148"/>
+      <c r="C11" s="149"/>
       <c r="D11" s="126">
         <f>SUM(D5:D10)</f>
         <v>9</v>
@@ -16496,7 +16490,7 @@
         <v>197</v>
       </c>
       <c r="D12" s="128">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F12" s="123"/>
       <c r="G12" s="117"/>
@@ -16520,7 +16514,7 @@
         <v>228</v>
       </c>
       <c r="D13" s="128">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F13" s="123"/>
       <c r="G13" s="117"/>
@@ -16544,7 +16538,7 @@
         <v>229</v>
       </c>
       <c r="D14" s="128">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F14" s="123"/>
       <c r="G14" s="117"/>
@@ -16568,7 +16562,7 @@
         <v>260</v>
       </c>
       <c r="D15" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="123"/>
       <c r="G15" s="117"/>
@@ -16592,7 +16586,7 @@
         <v>258</v>
       </c>
       <c r="D16" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="123"/>
       <c r="G16" s="117"/>
@@ -16616,7 +16610,7 @@
         <v>259</v>
       </c>
       <c r="D17" s="128">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F17" s="123"/>
       <c r="G17" s="117"/>
@@ -16640,7 +16634,7 @@
         <v>202</v>
       </c>
       <c r="D18" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="123"/>
       <c r="G18" s="117"/>
@@ -16664,7 +16658,7 @@
         <v>205</v>
       </c>
       <c r="D19" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="123"/>
       <c r="G19" s="117"/>
@@ -16688,7 +16682,7 @@
         <v>199</v>
       </c>
       <c r="D20" s="128">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -16709,7 +16703,7 @@
         <v>204</v>
       </c>
       <c r="D21" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
@@ -16720,14 +16714,14 @@
       <c r="L21" s="119"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="147"/>
-      <c r="C22" s="148"/>
+      <c r="B22" s="148"/>
+      <c r="C22" s="149"/>
       <c r="D22" s="126">
         <f>SUM(D12:D21)</f>
-        <v>25.5</v>
+        <v>61</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>
@@ -16748,7 +16742,7 @@
         <v>197</v>
       </c>
       <c r="D23" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23"/>
       <c r="G23"/>
@@ -16769,7 +16763,7 @@
         <v>261</v>
       </c>
       <c r="D24" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -16783,7 +16777,7 @@
         <v>192</v>
       </c>
       <c r="D25" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -16797,7 +16791,7 @@
         <v>230</v>
       </c>
       <c r="D26" s="128">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -16811,7 +16805,7 @@
         <v>241</v>
       </c>
       <c r="D27" s="128">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -16825,7 +16819,7 @@
         <v>242</v>
       </c>
       <c r="D28" s="128">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -16839,7 +16833,7 @@
         <v>262</v>
       </c>
       <c r="D29" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -16853,7 +16847,7 @@
         <v>209</v>
       </c>
       <c r="D30" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -16867,7 +16861,7 @@
         <v>206</v>
       </c>
       <c r="D31" s="128">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -16881,7 +16875,7 @@
         <v>208</v>
       </c>
       <c r="D32" s="128">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -16895,7 +16889,7 @@
         <v>207</v>
       </c>
       <c r="D33" s="128">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17011,14 +17005,14 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="146" t="s">
+      <c r="A46" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="147"/>
-      <c r="C46" s="148"/>
+      <c r="B46" s="148"/>
+      <c r="C46" s="149"/>
       <c r="D46" s="126">
         <f>SUM(D23:D45)</f>
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17032,7 +17026,7 @@
         <v>197</v>
       </c>
       <c r="D47" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17046,7 +17040,7 @@
         <v>210</v>
       </c>
       <c r="D48" s="128">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17060,7 +17054,7 @@
         <v>211</v>
       </c>
       <c r="D49" s="128">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17074,7 +17068,7 @@
         <v>216</v>
       </c>
       <c r="D50" s="128">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17088,7 +17082,7 @@
         <v>212</v>
       </c>
       <c r="D51" s="128">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17102,7 +17096,7 @@
         <v>213</v>
       </c>
       <c r="D52" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17116,7 +17110,7 @@
         <v>215</v>
       </c>
       <c r="D53" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17130,7 +17124,7 @@
         <v>214</v>
       </c>
       <c r="D54" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -17144,22 +17138,22 @@
         <v>199</v>
       </c>
       <c r="D55" s="128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A56" s="146"/>
-      <c r="B56" s="147"/>
-      <c r="C56" s="148"/>
+      <c r="A56" s="147"/>
+      <c r="B56" s="148"/>
+      <c r="C56" s="149"/>
       <c r="D56" s="126">
         <f>SUM(D47:D55)</f>
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="D57" s="137">
         <f>SUM(D11,D22,D46,D56)</f>
-        <v>90.5</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -17187,7 +17181,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17198,19 +17192,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
     </row>
     <row r="2" spans="1:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="160" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="159"/>
-      <c r="C3" s="159"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
@@ -17218,7 +17212,7 @@
       </c>
       <c r="B4" s="141">
         <f>'Backlog Produto'!$D$57</f>
-        <v>90.5</v>
+        <v>180</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>13</v>
@@ -17249,7 +17243,7 @@
         <v>231</v>
       </c>
       <c r="B7" s="15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>13</v>
@@ -17261,7 +17255,7 @@
       </c>
       <c r="B8" s="139">
         <f>B6*B7*2</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>13</v>
@@ -17273,7 +17267,7 @@
       </c>
       <c r="B9" s="138">
         <f>B11/2</f>
-        <v>5.65625</v>
+        <v>5.625</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>244</v>
@@ -17285,7 +17279,7 @@
       </c>
       <c r="B10" s="140">
         <f>B4+(B4*B5)</f>
-        <v>135.75</v>
+        <v>270</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>13</v>
@@ -17297,7 +17291,7 @@
       </c>
       <c r="B11" s="139">
         <f>B10/B8*2</f>
-        <v>11.3125</v>
+        <v>11.25</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>28</v>
@@ -17309,18 +17303,18 @@
       </c>
       <c r="B12" s="138">
         <f>B11/4</f>
-        <v>2.828125</v>
+        <v>2.8125</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="159" t="s">
+      <c r="A14" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="159"/>
-      <c r="C14" s="159"/>
+      <c r="B14" s="160"/>
+      <c r="C14" s="160"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -17337,7 +17331,7 @@
       </c>
       <c r="B16" s="5">
         <f>B10*B15</f>
-        <v>2715</v>
+        <v>5400</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -17366,7 +17360,7 @@
       </c>
       <c r="B19" s="142">
         <f>B16+B18</f>
-        <v>2715</v>
+        <v>5400</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -17385,7 +17379,7 @@
       </c>
       <c r="B21" s="7">
         <f>B19*B20</f>
-        <v>543</v>
+        <v>1080</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -17395,7 +17389,7 @@
       </c>
       <c r="B22" s="142">
         <f>B19+B21</f>
-        <v>3258</v>
+        <v>6480</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -17433,61 +17427,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="162"/>
+      <c r="J1" s="162"/>
+      <c r="K1" s="162"/>
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="163" t="s">
+      <c r="A2" s="164" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="165"/>
+      <c r="B2" s="166"/>
       <c r="C2" s="77">
         <v>2</v>
       </c>
-      <c r="D2" s="162" t="s">
+      <c r="D2" s="163" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="162"/>
+      <c r="E2" s="163"/>
       <c r="F2" s="78">
         <f>Planejamento!B9</f>
-        <v>5.65625</v>
-      </c>
-      <c r="G2" s="163" t="s">
+        <v>5.625</v>
+      </c>
+      <c r="G2" s="164" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164"/>
-      <c r="J2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="166"/>
       <c r="K2" s="77">
         <f>Planejamento!$B$10</f>
-        <v>135.75</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="79"/>
       <c r="B3" s="80"/>
-      <c r="C3" s="166" t="s">
+      <c r="C3" s="167" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
       <c r="F3" s="81"/>
-      <c r="G3" s="167" t="s">
+      <c r="G3" s="168" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="168"/>
-      <c r="I3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="170"/>
       <c r="J3" s="82"/>
       <c r="K3" s="83"/>
     </row>
@@ -18659,19 +18653,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="54" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="162"/>
+      <c r="J1" s="162"/>
+      <c r="K1" s="162"/>
     </row>
     <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="1:11" ht="12" hidden="1" x14ac:dyDescent="0.15">
@@ -18825,10 +18819,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D33" s="175" t="s">
+      <c r="D33" s="171" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="176"/>
+      <c r="E33" s="172"/>
     </row>
     <row r="34" spans="1:11" ht="12" hidden="1" x14ac:dyDescent="0.15">
       <c r="D34" s="62">
@@ -18880,137 +18874,137 @@
     </row>
     <row r="40" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="1:11" s="54" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="182" t="s">
+      <c r="A41" s="179" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="182"/>
-      <c r="C41" s="182"/>
-      <c r="D41" s="182"/>
-      <c r="E41" s="182"/>
-      <c r="F41" s="182"/>
-      <c r="G41" s="182"/>
-      <c r="H41" s="182"/>
-      <c r="I41" s="182"/>
-      <c r="J41" s="182"/>
-      <c r="K41" s="182"/>
+      <c r="B41" s="179"/>
+      <c r="C41" s="179"/>
+      <c r="D41" s="179"/>
+      <c r="E41" s="179"/>
+      <c r="F41" s="179"/>
+      <c r="G41" s="179"/>
+      <c r="H41" s="179"/>
+      <c r="I41" s="179"/>
+      <c r="J41" s="179"/>
+      <c r="K41" s="179"/>
     </row>
     <row r="42" spans="1:11" s="54" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="183" t="s">
+      <c r="A42" s="180" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="183"/>
-      <c r="C42" s="183"/>
-      <c r="D42" s="183"/>
-      <c r="E42" s="183"/>
-      <c r="F42" s="183"/>
-      <c r="G42" s="183"/>
-      <c r="H42" s="183"/>
-      <c r="I42" s="183"/>
-      <c r="J42" s="183"/>
-      <c r="K42" s="183"/>
+      <c r="B42" s="180"/>
+      <c r="C42" s="180"/>
+      <c r="D42" s="180"/>
+      <c r="E42" s="180"/>
+      <c r="F42" s="180"/>
+      <c r="G42" s="180"/>
+      <c r="H42" s="180"/>
+      <c r="I42" s="180"/>
+      <c r="J42" s="180"/>
+      <c r="K42" s="180"/>
     </row>
     <row r="43" spans="1:11" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="184" t="s">
+      <c r="A43" s="181" t="s">
         <v>134</v>
       </c>
-      <c r="B43" s="184"/>
-      <c r="C43" s="184"/>
-      <c r="D43" s="184"/>
-      <c r="E43" s="184"/>
-      <c r="F43" s="184"/>
-      <c r="G43" s="184"/>
-      <c r="H43" s="184"/>
-      <c r="I43" s="184"/>
-      <c r="J43" s="184"/>
-      <c r="K43" s="184"/>
+      <c r="B43" s="181"/>
+      <c r="C43" s="181"/>
+      <c r="D43" s="181"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="181"/>
+      <c r="G43" s="181"/>
+      <c r="H43" s="181"/>
+      <c r="I43" s="181"/>
+      <c r="J43" s="181"/>
+      <c r="K43" s="181"/>
     </row>
     <row r="44" spans="1:11" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="185" t="s">
+      <c r="A44" s="182" t="s">
         <v>121</v>
       </c>
-      <c r="B44" s="185"/>
-      <c r="C44" s="185"/>
-      <c r="D44" s="185"/>
-      <c r="E44" s="185"/>
-      <c r="F44" s="185"/>
-      <c r="G44" s="185"/>
-      <c r="H44" s="185"/>
-      <c r="I44" s="185"/>
-      <c r="J44" s="185"/>
-      <c r="K44" s="185"/>
+      <c r="B44" s="182"/>
+      <c r="C44" s="182"/>
+      <c r="D44" s="182"/>
+      <c r="E44" s="182"/>
+      <c r="F44" s="182"/>
+      <c r="G44" s="182"/>
+      <c r="H44" s="182"/>
+      <c r="I44" s="182"/>
+      <c r="J44" s="182"/>
+      <c r="K44" s="182"/>
     </row>
     <row r="45" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="46" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="177" t="s">
+      <c r="A46" s="173" t="s">
         <v>122</v>
       </c>
-      <c r="B46" s="178"/>
-      <c r="C46" s="178"/>
-      <c r="D46" s="178"/>
-      <c r="E46" s="178"/>
-      <c r="F46" s="178"/>
-      <c r="G46" s="178"/>
-      <c r="H46" s="178"/>
-      <c r="I46" s="178"/>
-      <c r="J46" s="178"/>
-      <c r="K46" s="178"/>
+      <c r="B46" s="174"/>
+      <c r="C46" s="174"/>
+      <c r="D46" s="174"/>
+      <c r="E46" s="174"/>
+      <c r="F46" s="174"/>
+      <c r="G46" s="174"/>
+      <c r="H46" s="174"/>
+      <c r="I46" s="174"/>
+      <c r="J46" s="174"/>
+      <c r="K46" s="174"/>
     </row>
     <row r="47" spans="1:11" s="66" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="76" t="s">
         <v>123</v>
       </c>
       <c r="B47" s="75"/>
-      <c r="C47" s="179" t="s">
+      <c r="C47" s="175" t="s">
         <v>124</v>
       </c>
-      <c r="D47" s="179"/>
-      <c r="E47" s="179"/>
-      <c r="F47" s="179"/>
-      <c r="G47" s="179"/>
-      <c r="H47" s="179"/>
-      <c r="I47" s="179"/>
-      <c r="J47" s="179"/>
-      <c r="K47" s="179"/>
+      <c r="D47" s="175"/>
+      <c r="E47" s="175"/>
+      <c r="F47" s="175"/>
+      <c r="G47" s="175"/>
+      <c r="H47" s="175"/>
+      <c r="I47" s="175"/>
+      <c r="J47" s="175"/>
+      <c r="K47" s="175"/>
     </row>
     <row r="48" spans="1:11" s="67" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="172"/>
-      <c r="B48" s="172" t="s">
+      <c r="A48" s="178"/>
+      <c r="B48" s="178" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="172" t="s">
+      <c r="C48" s="178" t="s">
         <v>125</v>
       </c>
-      <c r="D48" s="172" t="s">
+      <c r="D48" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="E48" s="172" t="s">
+      <c r="E48" s="178" t="s">
         <v>97</v>
       </c>
-      <c r="F48" s="172" t="s">
+      <c r="F48" s="178" t="s">
         <v>127</v>
       </c>
-      <c r="G48" s="172" t="s">
+      <c r="G48" s="178" t="s">
         <v>101</v>
       </c>
-      <c r="H48" s="173" t="s">
+      <c r="H48" s="185" t="s">
         <v>128</v>
       </c>
-      <c r="I48" s="174"/>
-      <c r="J48" s="174"/>
-      <c r="K48" s="174"/>
+      <c r="I48" s="186"/>
+      <c r="J48" s="186"/>
+      <c r="K48" s="186"/>
     </row>
     <row r="49" spans="1:11" s="67" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="172"/>
-      <c r="B49" s="172"/>
-      <c r="C49" s="172"/>
-      <c r="D49" s="172"/>
-      <c r="E49" s="172"/>
-      <c r="F49" s="172"/>
-      <c r="G49" s="172"/>
-      <c r="H49" s="180" t="s">
+      <c r="A49" s="178"/>
+      <c r="B49" s="178"/>
+      <c r="C49" s="178"/>
+      <c r="D49" s="178"/>
+      <c r="E49" s="178"/>
+      <c r="F49" s="178"/>
+      <c r="G49" s="178"/>
+      <c r="H49" s="176" t="s">
         <v>129</v>
       </c>
-      <c r="I49" s="181"/>
+      <c r="I49" s="177"/>
       <c r="J49" s="68" t="s">
         <v>130</v>
       </c>
@@ -19041,8 +19035,8 @@
       <c r="G50" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="H50" s="170"/>
-      <c r="I50" s="171"/>
+      <c r="H50" s="183"/>
+      <c r="I50" s="184"/>
       <c r="J50" s="74"/>
       <c r="K50" s="74" t="s">
         <v>136</v>
@@ -19199,8 +19193,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="G59" s="70"/>
-      <c r="H59" s="170"/>
-      <c r="I59" s="171"/>
+      <c r="H59" s="183"/>
+      <c r="I59" s="184"/>
       <c r="J59" s="74"/>
       <c r="K59" s="74"/>
     </row>
@@ -19215,13 +19209,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="G60" s="70"/>
-      <c r="H60" s="170"/>
-      <c r="I60" s="171"/>
+      <c r="H60" s="183"/>
+      <c r="I60" s="184"/>
       <c r="J60" s="74"/>
       <c r="K60" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:K48"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="A46:K46"/>
@@ -19233,15 +19236,6 @@
     <mergeCell ref="A42:K42"/>
     <mergeCell ref="A43:K43"/>
     <mergeCell ref="A44:K44"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:K48"/>
   </mergeCells>
   <conditionalFormatting sqref="F50:F60">
     <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
@@ -19292,20 +19286,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="187" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="79"/>
       <c r="B2" s="80"/>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="167" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="166"/>
+      <c r="D2" s="167"/>
     </row>
     <row r="3" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="84" t="s">
@@ -19438,7 +19432,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19495,7 +19489,7 @@
         <v>196</v>
       </c>
       <c r="B2" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -19513,7 +19507,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -19531,7 +19525,7 @@
         <v>193</v>
       </c>
       <c r="B4" s="15">
-        <v>5.5</v>
+        <v>11</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -19549,7 +19543,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -19567,7 +19561,7 @@
         <v>198</v>
       </c>
       <c r="B6" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -19585,7 +19579,7 @@
         <v>203</v>
       </c>
       <c r="B7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -19660,7 +19654,7 @@
       </c>
       <c r="B12" s="37">
         <f>SUM(B2:B11)</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="C12" s="37" t="str">
         <f>IF(SUM(C2:C11)&gt;0,B12-SUM(C2:C11), "")</f>
@@ -19710,43 +19704,43 @@
       </c>
       <c r="B13" s="34">
         <f>B12</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="C13" s="35">
         <f>B13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>8.5500000000000007</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="D13" s="35">
         <f t="shared" ref="D13:L13" si="1">C13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>7.6000000000000005</v>
+        <v>15.200000000000001</v>
       </c>
       <c r="E13" s="35">
         <f t="shared" si="1"/>
-        <v>6.65</v>
+        <v>13.3</v>
       </c>
       <c r="F13" s="35">
         <f t="shared" si="1"/>
-        <v>5.7</v>
+        <v>11.4</v>
       </c>
       <c r="G13" s="35">
         <f t="shared" si="1"/>
-        <v>4.75</v>
+        <v>9.5</v>
       </c>
       <c r="H13" s="35">
         <f t="shared" si="1"/>
-        <v>3.8</v>
+        <v>7.6</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" si="1"/>
-        <v>2.8499999999999996</v>
+        <v>5.6999999999999993</v>
       </c>
       <c r="J13" s="35">
         <f t="shared" si="1"/>
-        <v>1.8999999999999997</v>
+        <v>3.7999999999999994</v>
       </c>
       <c r="K13" s="35">
         <f t="shared" si="1"/>
-        <v>0.94999999999999973</v>
+        <v>1.8999999999999995</v>
       </c>
       <c r="L13" s="35">
         <f t="shared" si="1"/>
@@ -19759,47 +19753,47 @@
       </c>
       <c r="B14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="C14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="D14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="E14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="F14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="G14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="H14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="I14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="J14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="K14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="L14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -19857,7 +19851,7 @@
       </c>
       <c r="B16" s="43">
         <f>Planejamento!B8</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>12</v>
@@ -19884,7 +19878,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19941,7 +19935,7 @@
         <v>196</v>
       </c>
       <c r="B2" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -19959,7 +19953,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -19977,7 +19971,7 @@
         <v>193</v>
       </c>
       <c r="B4" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -19995,7 +19989,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -20013,7 +20007,7 @@
         <v>198</v>
       </c>
       <c r="B6" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -20031,7 +20025,7 @@
         <v>203</v>
       </c>
       <c r="B7" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -20106,7 +20100,7 @@
       </c>
       <c r="B12" s="37">
         <f>SUM(B2:B11)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C12" s="37" t="str">
         <f>IF(SUM(C2:C11)&gt;0,B12-SUM(C2:C11), "")</f>
@@ -20156,47 +20150,47 @@
       </c>
       <c r="B13" s="34">
         <f>B12</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13" s="35">
         <f>B13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>3.6</v>
+        <v>7.2</v>
       </c>
       <c r="D13" s="35">
         <f t="shared" ref="D13:L13" si="1">C13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>3.2</v>
+        <v>6.4</v>
       </c>
       <c r="E13" s="35">
         <f t="shared" si="1"/>
-        <v>2.8000000000000003</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="F13" s="35">
         <f t="shared" si="1"/>
-        <v>2.4000000000000004</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="G13" s="35">
         <f t="shared" si="1"/>
-        <v>2.0000000000000004</v>
+        <v>4.0000000000000009</v>
       </c>
       <c r="H13" s="35">
         <f t="shared" si="1"/>
-        <v>1.6000000000000005</v>
+        <v>3.2000000000000011</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" si="1"/>
-        <v>1.2000000000000006</v>
+        <v>2.4000000000000012</v>
       </c>
       <c r="J13" s="35">
         <f t="shared" si="1"/>
-        <v>0.8000000000000006</v>
+        <v>1.6000000000000012</v>
       </c>
       <c r="K13" s="35">
         <f t="shared" si="1"/>
-        <v>0.40000000000000058</v>
+        <v>0.80000000000000115</v>
       </c>
       <c r="L13" s="35">
         <f t="shared" si="1"/>
-        <v>5.5511151231257827E-16</v>
+        <v>1.1102230246251565E-15</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -20205,47 +20199,47 @@
       </c>
       <c r="B14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="C14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="D14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="E14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="F14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="G14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="H14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="I14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="J14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="K14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="L14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -20303,7 +20297,7 @@
       </c>
       <c r="B16" s="43">
         <f>Planejamento!B8</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>12</v>
@@ -20329,7 +20323,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20386,7 +20380,7 @@
         <v>196</v>
       </c>
       <c r="B2" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -20404,7 +20398,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -20422,7 +20416,7 @@
         <v>193</v>
       </c>
       <c r="B4" s="15">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -20440,7 +20434,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="15">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -20458,7 +20452,7 @@
         <v>198</v>
       </c>
       <c r="B6" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -20476,7 +20470,7 @@
         <v>203</v>
       </c>
       <c r="B7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -20551,7 +20545,7 @@
       </c>
       <c r="B12" s="37">
         <f>SUM(B2:B11)</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C12" s="37" t="str">
         <f>IF(SUM(C2:C11)&gt;0,B12-SUM(C2:C11), "")</f>
@@ -20601,43 +20595,43 @@
       </c>
       <c r="B13" s="34">
         <f>B12</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C13" s="35">
         <f>B13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>21.6</v>
+        <v>43.2</v>
       </c>
       <c r="D13" s="35">
         <f t="shared" ref="D13:L13" si="1">C13-($B$13/COUNTA($C$1:$L$1))</f>
-        <v>19.200000000000003</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="E13" s="35">
         <f t="shared" si="1"/>
-        <v>16.800000000000004</v>
+        <v>33.600000000000009</v>
       </c>
       <c r="F13" s="35">
         <f t="shared" si="1"/>
-        <v>14.400000000000004</v>
+        <v>28.800000000000008</v>
       </c>
       <c r="G13" s="35">
         <f t="shared" si="1"/>
-        <v>12.000000000000004</v>
+        <v>24.000000000000007</v>
       </c>
       <c r="H13" s="35">
         <f t="shared" si="1"/>
-        <v>9.6000000000000032</v>
+        <v>19.200000000000006</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" si="1"/>
-        <v>7.2000000000000028</v>
+        <v>14.400000000000006</v>
       </c>
       <c r="J13" s="35">
         <f t="shared" si="1"/>
-        <v>4.8000000000000025</v>
+        <v>9.600000000000005</v>
       </c>
       <c r="K13" s="35">
         <f t="shared" si="1"/>
-        <v>2.4000000000000026</v>
+        <v>4.8000000000000052</v>
       </c>
       <c r="L13" s="35">
         <f t="shared" si="1"/>
@@ -20650,47 +20644,47 @@
       </c>
       <c r="B14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="C14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="D14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="E14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="F14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="G14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="H14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="I14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="J14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="K14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
       <c r="L14" s="39">
         <f ca="1">OFFSET(Sprint1!$B$12,0,0,1,COUNT(Sprint1!$B$12:$L$12))</f>
-        <v>9.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -20748,7 +20742,7 @@
       </c>
       <c r="B16" s="43">
         <f>Planejamento!B8</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Modificacoes nos documentos visao e planilha de planejamento
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/Planejamento e Controle do epCafe.xlsx
+++ b/Gerenciamento de Projeto/Planejamento e Controle do epCafe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Documents/Java/grupo-6/Gerenciamento de Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC72D3B-4A9A-B048-9D84-2EA778A1F6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8379968-D69C-774B-9367-8CE8C5E7E028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" tabRatio="797" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="10" r:id="rId1"/>
@@ -3420,7 +3420,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="273">
   <si>
     <t>Iniciação</t>
   </si>
@@ -4319,6 +4319,12 @@
   </si>
   <si>
     <t>Indisponibilidade de Reurso</t>
+  </si>
+  <si>
+    <t>Iago Pereira de Barros</t>
+  </si>
+  <si>
+    <t>iagopereira72@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -5072,7 +5078,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5571,6 +5577,21 @@
     <xf numFmtId="0" fontId="28" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5592,9 +5613,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5606,18 +5624,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5667,6 +5673,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
@@ -13463,8 +13470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13555,9 +13562,15 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
+      <c r="A9" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="203" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
@@ -13610,9 +13623,10 @@
     <hyperlink ref="C8" r:id="rId3" xr:uid="{58049A4D-C39C-3846-9E52-245C24A91647}"/>
     <hyperlink ref="C7" r:id="rId4" xr:uid="{4B9B976D-E77B-524D-932A-14B75BD3E3FA}"/>
     <hyperlink ref="C4" r:id="rId5" xr:uid="{9824BE92-A973-114B-9257-FE5D79E5D8BD}"/>
+    <hyperlink ref="C9" r:id="rId6" display="mailto:iagopereira72@gmail.com" xr:uid="{F2FA135B-9769-594B-A663-CAC03C448081}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <legacyDrawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -16175,7 +16189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -18819,10 +18833,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D33" s="171" t="s">
+      <c r="D33" s="176" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="172"/>
+      <c r="E33" s="177"/>
     </row>
     <row r="34" spans="1:11" ht="12" hidden="1" x14ac:dyDescent="0.15">
       <c r="D34" s="62">
@@ -18874,137 +18888,137 @@
     </row>
     <row r="40" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="1:11" s="54" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="179" t="s">
+      <c r="A41" s="183" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="179"/>
-      <c r="C41" s="179"/>
-      <c r="D41" s="179"/>
-      <c r="E41" s="179"/>
-      <c r="F41" s="179"/>
-      <c r="G41" s="179"/>
-      <c r="H41" s="179"/>
-      <c r="I41" s="179"/>
-      <c r="J41" s="179"/>
-      <c r="K41" s="179"/>
+      <c r="B41" s="183"/>
+      <c r="C41" s="183"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="183"/>
+      <c r="F41" s="183"/>
+      <c r="G41" s="183"/>
+      <c r="H41" s="183"/>
+      <c r="I41" s="183"/>
+      <c r="J41" s="183"/>
+      <c r="K41" s="183"/>
     </row>
     <row r="42" spans="1:11" s="54" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="180" t="s">
+      <c r="A42" s="184" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="180"/>
-      <c r="C42" s="180"/>
-      <c r="D42" s="180"/>
-      <c r="E42" s="180"/>
-      <c r="F42" s="180"/>
-      <c r="G42" s="180"/>
-      <c r="H42" s="180"/>
-      <c r="I42" s="180"/>
-      <c r="J42" s="180"/>
-      <c r="K42" s="180"/>
+      <c r="B42" s="184"/>
+      <c r="C42" s="184"/>
+      <c r="D42" s="184"/>
+      <c r="E42" s="184"/>
+      <c r="F42" s="184"/>
+      <c r="G42" s="184"/>
+      <c r="H42" s="184"/>
+      <c r="I42" s="184"/>
+      <c r="J42" s="184"/>
+      <c r="K42" s="184"/>
     </row>
     <row r="43" spans="1:11" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="181" t="s">
+      <c r="A43" s="185" t="s">
         <v>134</v>
       </c>
-      <c r="B43" s="181"/>
-      <c r="C43" s="181"/>
-      <c r="D43" s="181"/>
-      <c r="E43" s="181"/>
-      <c r="F43" s="181"/>
-      <c r="G43" s="181"/>
-      <c r="H43" s="181"/>
-      <c r="I43" s="181"/>
-      <c r="J43" s="181"/>
-      <c r="K43" s="181"/>
+      <c r="B43" s="185"/>
+      <c r="C43" s="185"/>
+      <c r="D43" s="185"/>
+      <c r="E43" s="185"/>
+      <c r="F43" s="185"/>
+      <c r="G43" s="185"/>
+      <c r="H43" s="185"/>
+      <c r="I43" s="185"/>
+      <c r="J43" s="185"/>
+      <c r="K43" s="185"/>
     </row>
     <row r="44" spans="1:11" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="182" t="s">
+      <c r="A44" s="186" t="s">
         <v>121</v>
       </c>
-      <c r="B44" s="182"/>
-      <c r="C44" s="182"/>
-      <c r="D44" s="182"/>
-      <c r="E44" s="182"/>
-      <c r="F44" s="182"/>
-      <c r="G44" s="182"/>
-      <c r="H44" s="182"/>
-      <c r="I44" s="182"/>
-      <c r="J44" s="182"/>
-      <c r="K44" s="182"/>
+      <c r="B44" s="186"/>
+      <c r="C44" s="186"/>
+      <c r="D44" s="186"/>
+      <c r="E44" s="186"/>
+      <c r="F44" s="186"/>
+      <c r="G44" s="186"/>
+      <c r="H44" s="186"/>
+      <c r="I44" s="186"/>
+      <c r="J44" s="186"/>
+      <c r="K44" s="186"/>
     </row>
     <row r="45" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="46" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="173" t="s">
+      <c r="A46" s="178" t="s">
         <v>122</v>
       </c>
-      <c r="B46" s="174"/>
-      <c r="C46" s="174"/>
-      <c r="D46" s="174"/>
-      <c r="E46" s="174"/>
-      <c r="F46" s="174"/>
-      <c r="G46" s="174"/>
-      <c r="H46" s="174"/>
-      <c r="I46" s="174"/>
-      <c r="J46" s="174"/>
-      <c r="K46" s="174"/>
+      <c r="B46" s="179"/>
+      <c r="C46" s="179"/>
+      <c r="D46" s="179"/>
+      <c r="E46" s="179"/>
+      <c r="F46" s="179"/>
+      <c r="G46" s="179"/>
+      <c r="H46" s="179"/>
+      <c r="I46" s="179"/>
+      <c r="J46" s="179"/>
+      <c r="K46" s="179"/>
     </row>
     <row r="47" spans="1:11" s="66" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="76" t="s">
         <v>123</v>
       </c>
       <c r="B47" s="75"/>
-      <c r="C47" s="175" t="s">
+      <c r="C47" s="180" t="s">
         <v>124</v>
       </c>
-      <c r="D47" s="175"/>
-      <c r="E47" s="175"/>
-      <c r="F47" s="175"/>
-      <c r="G47" s="175"/>
-      <c r="H47" s="175"/>
-      <c r="I47" s="175"/>
-      <c r="J47" s="175"/>
-      <c r="K47" s="175"/>
+      <c r="D47" s="180"/>
+      <c r="E47" s="180"/>
+      <c r="F47" s="180"/>
+      <c r="G47" s="180"/>
+      <c r="H47" s="180"/>
+      <c r="I47" s="180"/>
+      <c r="J47" s="180"/>
+      <c r="K47" s="180"/>
     </row>
     <row r="48" spans="1:11" s="67" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="178"/>
-      <c r="B48" s="178" t="s">
+      <c r="A48" s="173"/>
+      <c r="B48" s="173" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="178" t="s">
+      <c r="C48" s="173" t="s">
         <v>125</v>
       </c>
-      <c r="D48" s="178" t="s">
+      <c r="D48" s="173" t="s">
         <v>126</v>
       </c>
-      <c r="E48" s="178" t="s">
+      <c r="E48" s="173" t="s">
         <v>97</v>
       </c>
-      <c r="F48" s="178" t="s">
+      <c r="F48" s="173" t="s">
         <v>127</v>
       </c>
-      <c r="G48" s="178" t="s">
+      <c r="G48" s="173" t="s">
         <v>101</v>
       </c>
-      <c r="H48" s="185" t="s">
+      <c r="H48" s="174" t="s">
         <v>128</v>
       </c>
-      <c r="I48" s="186"/>
-      <c r="J48" s="186"/>
-      <c r="K48" s="186"/>
+      <c r="I48" s="175"/>
+      <c r="J48" s="175"/>
+      <c r="K48" s="175"/>
     </row>
     <row r="49" spans="1:11" s="67" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="178"/>
-      <c r="B49" s="178"/>
-      <c r="C49" s="178"/>
-      <c r="D49" s="178"/>
-      <c r="E49" s="178"/>
-      <c r="F49" s="178"/>
-      <c r="G49" s="178"/>
-      <c r="H49" s="176" t="s">
+      <c r="A49" s="173"/>
+      <c r="B49" s="173"/>
+      <c r="C49" s="173"/>
+      <c r="D49" s="173"/>
+      <c r="E49" s="173"/>
+      <c r="F49" s="173"/>
+      <c r="G49" s="173"/>
+      <c r="H49" s="181" t="s">
         <v>129</v>
       </c>
-      <c r="I49" s="177"/>
+      <c r="I49" s="182"/>
       <c r="J49" s="68" t="s">
         <v>130</v>
       </c>
@@ -19035,8 +19049,8 @@
       <c r="G50" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="H50" s="183"/>
-      <c r="I50" s="184"/>
+      <c r="H50" s="171"/>
+      <c r="I50" s="172"/>
       <c r="J50" s="74"/>
       <c r="K50" s="74" t="s">
         <v>136</v>
@@ -19193,8 +19207,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="G59" s="70"/>
-      <c r="H59" s="183"/>
-      <c r="I59" s="184"/>
+      <c r="H59" s="171"/>
+      <c r="I59" s="172"/>
       <c r="J59" s="74"/>
       <c r="K59" s="74"/>
     </row>
@@ -19209,22 +19223,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="G60" s="70"/>
-      <c r="H60" s="183"/>
-      <c r="I60" s="184"/>
+      <c r="H60" s="171"/>
+      <c r="I60" s="172"/>
       <c r="J60" s="74"/>
       <c r="K60" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:K48"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="A46:K46"/>
@@ -19236,6 +19241,15 @@
     <mergeCell ref="A42:K42"/>
     <mergeCell ref="A43:K43"/>
     <mergeCell ref="A44:K44"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:K48"/>
   </mergeCells>
   <conditionalFormatting sqref="F50:F60">
     <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>